<commit_message>
Adding to notes file where indices are loaded.
</commit_message>
<xml_diff>
--- a/OldVersions_Setup_LitReview/From_Config/HPV_parameters_HPV.xlsx
+++ b/OldVersions_Setup_LitReview/From_Config/HPV_parameters_HPV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CISNET\HHCoM\OldVersions_SetupFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CISNET\HHCoM\OldVersions_Setup_LitReview\From_Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>Annual Transition Rate</t>
   </si>
@@ -138,33 +138,6 @@
   </si>
   <si>
     <t>High</t>
-  </si>
-  <si>
-    <t>HPV Prevalence and Odds Ratios when HIV positive</t>
-  </si>
-  <si>
-    <t>Covariate</t>
-  </si>
-  <si>
-    <t>Adjusted Odds Ratio</t>
-  </si>
-  <si>
-    <t>HIV negative</t>
-  </si>
-  <si>
-    <t>HIV positive: CD4 &gt; 200, RNA &lt; 20,000 copies/mL</t>
-  </si>
-  <si>
-    <t>HIV positive: CD4 &gt; 200 , RNA &gt; 20000 copes/mL</t>
-  </si>
-  <si>
-    <t>HIV positve CD4 &lt; 200</t>
-  </si>
-  <si>
-    <t>Palefsky et al. (1999 , JNCI)</t>
-  </si>
-  <si>
-    <t>Reflects persistence/reactivation of pre-existing HPV types</t>
   </si>
   <si>
     <t>SA</t>
@@ -375,16 +348,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -679,7 +652,7 @@
     <col min="13" max="13" width="49.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -691,14 +664,14 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="1"/>
-      <c r="M1" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L1" s="38"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -708,12 +681,14 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="1"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L2" s="38"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -739,20 +714,14 @@
         <v>4</v>
       </c>
       <c r="I3" s="1"/>
-      <c r="M3" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="34" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L3" s="38"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="38"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -778,20 +747,14 @@
         <v>0.04</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="M4" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" s="35">
-        <v>1</v>
-      </c>
-      <c r="O4" s="33">
-        <v>1</v>
-      </c>
-      <c r="P4" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -817,20 +780,14 @@
         <v>0.192</v>
       </c>
       <c r="I5" s="1"/>
-      <c r="M5" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="33">
-        <v>3.12</v>
-      </c>
-      <c r="O5" s="33">
-        <v>2.36</v>
-      </c>
-      <c r="P5" s="33">
-        <v>4.12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -854,20 +811,14 @@
         <v>0.27600000000000002</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="M6" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="N6" s="33">
-        <v>5.78</v>
-      </c>
-      <c r="O6" s="33">
-        <v>4.17</v>
-      </c>
-      <c r="P6" s="33">
-        <v>8.08</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -889,20 +840,14 @@
       <c r="I7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="33">
-        <v>10.130000000000001</v>
-      </c>
-      <c r="O7" s="33">
-        <v>7.32</v>
-      </c>
-      <c r="P7" s="33">
-        <v>14.04</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -928,14 +873,14 @@
         <v>1.645</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="M8" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L8" s="38"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -961,14 +906,22 @@
         <v>0.82199999999999995</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="M9" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L9" s="38"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -977,7 +930,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>12</v>
       </c>
@@ -987,14 +940,14 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="O12" s="37"/>
-      <c r="P12" s="37"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M12" s="34"/>
+      <c r="N12" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>13</v>
       </c>
@@ -1014,16 +967,16 @@
       <c r="G13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="N13" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
@@ -1043,20 +996,20 @@
       <c r="G14" s="9">
         <v>0.75774999999999992</v>
       </c>
-      <c r="M14" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="N14" s="37">
+      <c r="M14" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="34">
         <v>0.91</v>
       </c>
-      <c r="O14" s="37">
+      <c r="O14" s="34">
         <v>0.28000000000000003</v>
       </c>
-      <c r="P14" s="37">
+      <c r="P14" s="34">
         <v>2.92</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
@@ -1076,20 +1029,20 @@
       <c r="G15" s="9">
         <v>1</v>
       </c>
-      <c r="M15" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="N15" s="37">
+      <c r="M15" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" s="34">
         <v>1.2</v>
       </c>
-      <c r="O15" s="37">
+      <c r="O15" s="34">
         <v>0.88</v>
       </c>
-      <c r="P15" s="37">
+      <c r="P15" s="34">
         <v>1.64</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
@@ -1105,16 +1058,16 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="M16" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="N16" s="37">
+      <c r="M16" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="N16" s="34">
         <v>1.32</v>
       </c>
-      <c r="O16" s="37">
+      <c r="O16" s="34">
         <v>0.85</v>
       </c>
-      <c r="P16" s="37">
+      <c r="P16" s="34">
         <v>2.06</v>
       </c>
     </row>
@@ -1131,14 +1084,14 @@
       <c r="D17" s="9">
         <v>1.7130000000000001</v>
       </c>
-      <c r="M17" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="N17" s="37">
+      <c r="M17" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="N17" s="34">
         <v>1</v>
       </c>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
@@ -1153,10 +1106,10 @@
       <c r="D18" s="10">
         <v>1.863</v>
       </c>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
@@ -1171,12 +1124,12 @@
       <c r="D19" s="10">
         <v>1.458</v>
       </c>
-      <c r="M19" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
+      <c r="M19" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
@@ -1191,14 +1144,14 @@
       <c r="D20" s="10">
         <v>1.679</v>
       </c>
-      <c r="M20" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="N20" s="37">
+      <c r="M20" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="N20" s="34">
         <v>1</v>
       </c>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
@@ -1207,30 +1160,30 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="M21" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="N21" s="37">
+      <c r="M21" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="N21" s="34">
         <v>1.75</v>
       </c>
-      <c r="O21" s="37">
+      <c r="O21" s="34">
         <v>1.1599999999999999</v>
       </c>
-      <c r="P21" s="37">
+      <c r="P21" s="34">
         <v>2.65</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="M22" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="N22" s="37">
+      <c r="M22" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="N22" s="34">
         <v>1.68</v>
       </c>
-      <c r="O22" s="37">
+      <c r="O22" s="34">
         <v>1.02</v>
       </c>
-      <c r="P22" s="37">
+      <c r="P22" s="34">
         <v>2.79</v>
       </c>
     </row>
@@ -1239,10 +1192,10 @@
         <v>25</v>
       </c>
       <c r="B23" s="13"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
@@ -1259,41 +1212,41 @@
       <c r="B25" s="14">
         <v>0.49382716049382713</v>
       </c>
-      <c r="M25" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
+      <c r="M25" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="M26" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="N26" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="O26" s="39" t="s">
+      <c r="M26" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="N26" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="O26" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="P26" s="39" t="s">
+      <c r="P26" s="36" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="M27" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="N27" s="33">
+      <c r="M27" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="N27" s="32">
         <v>0.43</v>
       </c>
-      <c r="O27" s="33">
+      <c r="O27" s="32">
         <v>0.39</v>
       </c>
-      <c r="P27" s="33">
+      <c r="P27" s="32">
         <v>0.47</v>
       </c>
     </row>
@@ -1303,16 +1256,16 @@
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
-      <c r="M28" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="N28" s="33">
+      <c r="M28" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="N28" s="32">
         <v>0.28999999999999998</v>
       </c>
-      <c r="O28" s="33">
+      <c r="O28" s="32">
         <v>0.24</v>
       </c>
-      <c r="P28" s="33">
+      <c r="P28" s="32">
         <v>0.34</v>
       </c>
     </row>
@@ -1324,10 +1277,10 @@
       <c r="C29" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="37"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="34"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
@@ -1339,12 +1292,12 @@
       <c r="C30" s="22">
         <v>0.75774999999999992</v>
       </c>
-      <c r="M30" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="N30" s="37"/>
-      <c r="O30" s="37"/>
-      <c r="P30" s="37"/>
+      <c r="M30" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
+      <c r="P30" s="34"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="19" t="s">
@@ -1356,12 +1309,12 @@
       <c r="C31" s="22">
         <v>1</v>
       </c>
-      <c r="M31" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="N31" s="37"/>
-      <c r="O31" s="37"/>
-      <c r="P31" s="37"/>
+      <c r="M31" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="N31" s="34"/>
+      <c r="O31" s="34"/>
+      <c r="P31" s="34"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="20" t="s">
@@ -1384,12 +1337,12 @@
       <c r="E34" s="23"/>
       <c r="F34" s="23"/>
       <c r="G34" s="23"/>
-      <c r="M34" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="N34" s="37"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="37"/>
+      <c r="M34" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="N34" s="34"/>
+      <c r="O34" s="34"/>
+      <c r="P34" s="34"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="26" t="s">
@@ -1411,16 +1364,16 @@
       <c r="G35" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="M35" s="39" t="s">
+      <c r="M35" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="N35" s="39" t="s">
+      <c r="N35" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="O35" s="39" t="s">
+      <c r="O35" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="P35" s="39" t="s">
+      <c r="P35" s="36" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1444,16 +1397,16 @@
       <c r="G36" s="25">
         <v>1.925E-2</v>
       </c>
-      <c r="M36" s="33">
+      <c r="M36" s="32">
         <v>16</v>
       </c>
-      <c r="N36" s="33">
+      <c r="N36" s="32">
         <v>0.755</v>
       </c>
-      <c r="O36" s="33">
+      <c r="O36" s="32">
         <v>0.29499999999999998</v>
       </c>
-      <c r="P36" s="33">
+      <c r="P36" s="32">
         <v>1</v>
       </c>
     </row>
@@ -1477,16 +1430,16 @@
       <c r="G37" s="25">
         <v>1.9E-2</v>
       </c>
-      <c r="M37" s="33">
+      <c r="M37" s="32">
         <v>18</v>
       </c>
-      <c r="N37" s="33">
+      <c r="N37" s="32">
         <v>0.73599999999999999</v>
       </c>
-      <c r="O37" s="33">
+      <c r="O37" s="32">
         <v>0.29199999999999998</v>
       </c>
-      <c r="P37" s="33">
+      <c r="P37" s="32">
         <v>1</v>
       </c>
     </row>
@@ -1510,10 +1463,10 @@
       <c r="G38" s="25">
         <v>1.925E-2</v>
       </c>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33"/>
-      <c r="O38" s="33"/>
-      <c r="P38" s="33"/>
+      <c r="M38" s="32"/>
+      <c r="N38" s="32"/>
+      <c r="O38" s="32"/>
+      <c r="P38" s="32"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="24" t="s">
@@ -1531,16 +1484,16 @@
       <c r="E39" s="23"/>
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
-      <c r="M39" s="33">
+      <c r="M39" s="32">
         <v>39</v>
       </c>
-      <c r="N39" s="33">
+      <c r="N39" s="32">
         <v>0.755</v>
       </c>
-      <c r="O39" s="33">
+      <c r="O39" s="32">
         <v>0.23300000000000001</v>
       </c>
-      <c r="P39" s="33">
+      <c r="P39" s="32">
         <v>1</v>
       </c>
     </row>
@@ -1560,16 +1513,16 @@
       <c r="E40" s="23"/>
       <c r="F40" s="23"/>
       <c r="G40" s="23"/>
-      <c r="M40" s="33">
+      <c r="M40" s="32">
         <v>51</v>
       </c>
-      <c r="N40" s="33">
+      <c r="N40" s="32">
         <v>0.755</v>
       </c>
-      <c r="O40" s="33">
+      <c r="O40" s="32">
         <v>0.23300000000000001</v>
       </c>
-      <c r="P40" s="33">
+      <c r="P40" s="32">
         <v>1</v>
       </c>
     </row>
@@ -1589,16 +1542,16 @@
       <c r="E41" s="23"/>
       <c r="F41" s="23"/>
       <c r="G41" s="23"/>
-      <c r="M41" s="33">
+      <c r="M41" s="32">
         <v>56</v>
       </c>
-      <c r="N41" s="33">
+      <c r="N41" s="32">
         <v>0.74299999999999999</v>
       </c>
-      <c r="O41" s="33">
+      <c r="O41" s="32">
         <v>0.253</v>
       </c>
-      <c r="P41" s="33">
+      <c r="P41" s="32">
         <v>1</v>
       </c>
     </row>
@@ -1615,20 +1568,20 @@
       <c r="D42" s="25">
         <v>0.113</v>
       </c>
-      <c r="M42" s="37"/>
-      <c r="N42" s="37"/>
-      <c r="O42" s="37"/>
-      <c r="P42" s="37"/>
+      <c r="M42" s="34"/>
+      <c r="N42" s="34"/>
+      <c r="O42" s="34"/>
+      <c r="P42" s="34"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="M43" s="39" t="s">
+      <c r="M43" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="N43" s="39" t="s">
+      <c r="N43" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="O43" s="37"/>
-      <c r="P43" s="37"/>
+      <c r="O43" s="34"/>
+      <c r="P43" s="34"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="30" t="s">
@@ -1636,15 +1589,15 @@
       </c>
       <c r="B44" s="28"/>
       <c r="C44" s="28"/>
-      <c r="M44" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="N44" s="33">
+      <c r="M44" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="N44" s="32">
         <f>AVERAGE(N36:N37)</f>
         <v>0.74550000000000005</v>
       </c>
-      <c r="O44" s="37"/>
-      <c r="P44" s="37"/>
+      <c r="O44" s="34"/>
+      <c r="P44" s="34"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="29" t="s">
@@ -1656,15 +1609,15 @@
       <c r="C45" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="M45" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="N45" s="33">
+      <c r="M45" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="N45" s="32">
         <f>AVERAGE(N39:N41)</f>
         <v>0.751</v>
       </c>
-      <c r="O45" s="37"/>
-      <c r="P45" s="37"/>
+      <c r="O45" s="34"/>
+      <c r="P45" s="34"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="29">
@@ -1678,118 +1631,118 @@
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="M48" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="N48" s="37"/>
-      <c r="O48" s="37"/>
-      <c r="P48" s="37"/>
+      <c r="M48" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="N48" s="34"/>
+      <c r="O48" s="34"/>
+      <c r="P48" s="34"/>
     </row>
     <row r="49" spans="13:16" x14ac:dyDescent="0.35">
-      <c r="M49" s="37"/>
-      <c r="N49" s="37"/>
-      <c r="O49" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="P49" s="37" t="s">
-        <v>75</v>
+      <c r="M49" s="34"/>
+      <c r="N49" s="34"/>
+      <c r="O49" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="P49" s="34" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="13:16" x14ac:dyDescent="0.35">
-      <c r="M50" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="N50" s="37">
+      <c r="M50" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="N50" s="34">
         <v>15.5813953488371</v>
       </c>
-      <c r="O50" s="37">
+      <c r="O50" s="34">
         <v>14.5348837209302</v>
       </c>
-      <c r="P50" s="37">
+      <c r="P50" s="34">
         <v>16.6279069767441</v>
       </c>
     </row>
     <row r="51" spans="13:16" x14ac:dyDescent="0.35">
-      <c r="M51" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="N51" s="37">
+      <c r="M51" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="N51" s="34">
         <v>37.209302325581298</v>
       </c>
-      <c r="O51" s="37">
+      <c r="O51" s="34">
         <v>34.767441860465098</v>
       </c>
-      <c r="P51" s="37">
+      <c r="P51" s="34">
         <v>39.999999999999901</v>
       </c>
     </row>
     <row r="52" spans="13:16" x14ac:dyDescent="0.35">
-      <c r="M52" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="N52" s="37">
+      <c r="M52" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="N52" s="34">
         <v>43.139534883720899</v>
       </c>
-      <c r="O52" s="37">
+      <c r="O52" s="34">
         <v>41.395348837209298</v>
       </c>
-      <c r="P52" s="37">
+      <c r="P52" s="34">
         <v>45.232558139534802</v>
       </c>
     </row>
     <row r="53" spans="13:16" x14ac:dyDescent="0.35">
-      <c r="M53" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="N53" s="37">
+      <c r="M53" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="N53" s="34">
         <v>41.395348837209298</v>
       </c>
-      <c r="O53" s="37">
+      <c r="O53" s="34">
         <v>38.953488372092998</v>
       </c>
-      <c r="P53" s="37">
+      <c r="P53" s="34">
         <v>43.139534883720899</v>
       </c>
     </row>
     <row r="54" spans="13:16" x14ac:dyDescent="0.35">
-      <c r="M54" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="N54" s="37">
+      <c r="M54" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="N54" s="34">
         <v>37.906976744185997</v>
       </c>
-      <c r="O54" s="37">
+      <c r="O54" s="34">
         <v>36.511627906976699</v>
       </c>
-      <c r="P54" s="37">
+      <c r="P54" s="34">
         <v>39.651162790697597</v>
       </c>
     </row>
     <row r="55" spans="13:16" x14ac:dyDescent="0.35">
-      <c r="M55" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="N55" s="37">
+      <c r="M55" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="N55" s="34">
         <v>22.558139534883701</v>
       </c>
-      <c r="O55" s="37">
+      <c r="O55" s="34">
         <v>19.767441860465102</v>
       </c>
-      <c r="P55" s="37">
+      <c r="P55" s="34">
         <v>24.651162790697601</v>
       </c>
     </row>
     <row r="56" spans="13:16" x14ac:dyDescent="0.35">
-      <c r="M56" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="N56" s="37">
+      <c r="M56" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="N56" s="34">
         <v>13.4883720930232</v>
       </c>
-      <c r="O56" s="37">
+      <c r="O56" s="34">
         <v>12.0930232558139</v>
       </c>
-      <c r="P56" s="37">
+      <c r="P56" s="34">
         <v>14.883720930232499</v>
       </c>
     </row>

</xml_diff>